<commit_message>
Refactor code and Constriction parser working.
It has no validations.
</commit_message>
<xml_diff>
--- a/files/v6 (junio-julio).xlsx
+++ b/files/v6 (junio-julio).xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FDCCBA-9C3E-4495-88C4-F739992D61B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC77A2C-7516-416E-AC2E-5C63F1A6B167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="datos" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="capacidades" sheetId="5" r:id="rId4"/>
-    <sheet name="ListaExámenes2020-2021paraCSV" sheetId="6" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="datos" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="capacidades" sheetId="5" r:id="rId5"/>
+    <sheet name="ListaExámenes2020-2021paraCSV" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">planificación!$A$5:$P$67</definedName>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="383">
   <si>
     <t>ID</t>
   </si>
@@ -1247,6 +1248,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1856,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1897,6 +1914,27 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1951,23 +1989,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2272,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6142,17 +6180,17 @@
     <mergeCell ref="O5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:P9 A10:O10 A35:P67 A34:O34 A11:P33">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="23" priority="15">
       <formula>$Q6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6:O67">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6163,6 +6201,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="30">
+        <v>44553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>$Q1=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="expression" dxfId="19" priority="3">
+      <formula>$Q2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="18" priority="2">
+      <formula>$Q3=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$Q3=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
@@ -7727,7 +7836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:C18"/>
   <sheetViews>
@@ -7878,7 +7987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:O30"/>
   <sheetViews>
@@ -8522,7 +8631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I281"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added configurations files using resources.
Also changed configurations in the project for the IDE. These changes imply some files moving, as are the test ones.
</commit_message>
<xml_diff>
--- a/files/v6 (junio-julio).xlsx
+++ b/files/v6 (junio-julio).xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC77A2C-7516-416E-AC2E-5C63F1A6B167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF8699D-F88D-4B32-B0A4-A20540177A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="2175" windowWidth="26430" windowHeight="13335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="datos" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="capacidades" sheetId="5" r:id="rId5"/>
-    <sheet name="ListaExámenes2020-2021paraCSV" sheetId="6" r:id="rId6"/>
+    <sheet name="Restricciones de Usuario" sheetId="7" r:id="rId2"/>
+    <sheet name="Calendario fechas" sheetId="8" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="datos" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="capacidades" sheetId="5" r:id="rId6"/>
+    <sheet name="ListaExámenes2020-2021paraCSV" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">planificación!$A$5:$P$67</definedName>
@@ -1858,13 +1859,6 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1914,6 +1908,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1989,23 +1990,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6205,7 +6206,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6263,7 +6264,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$Q3=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6272,6 +6273,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A3CB9E-ED1A-40D2-8190-0A166B48A835}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30">
+        <v>44240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>44269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
@@ -7836,7 +7862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:C18"/>
   <sheetViews>
@@ -7987,7 +8013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:O30"/>
   <sheetViews>
@@ -8631,7 +8657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I281"/>
   <sheetViews>

</xml_diff>